<commit_message>
test case 600 modified
</commit_message>
<xml_diff>
--- a/test_files/Codelist_with_def_hierarchy_extensions_and_members.xlsx
+++ b/test_files/Codelist_with_def_hierarchy_extensions_and_members.xlsx
@@ -15,20 +15,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="162">
   <si>
     <t>CODEVALUE</t>
   </si>
   <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>PROPERTYTYPE</t>
+  </si>
+  <si>
+    <t>CODESCHEMES</t>
+  </si>
+  <si>
+    <t>PREFLABEL_FI</t>
+  </si>
+  <si>
+    <t>PREFLABEL_EN</t>
+  </si>
+  <si>
+    <t>STARTDATE</t>
+  </si>
+  <si>
+    <t>ENDDATE</t>
+  </si>
+  <si>
+    <t>MEMBERSSHEET</t>
+  </si>
+  <si>
+    <t>O1234567890123456789012345678901234567111</t>
+  </si>
+  <si>
+    <t>DRAFT</t>
+  </si>
+  <si>
+    <t>definitionHierarchy</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/eu/dcat</t>
+  </si>
+  <si>
     <t>CLASSIFICATION</t>
   </si>
   <si>
     <t>VERSION</t>
   </si>
   <si>
-    <t>STATUS</t>
-  </si>
-  <si>
     <t>SOURCE</t>
   </si>
   <si>
@@ -41,18 +74,6 @@
     <t>DEFAULTCODE</t>
   </si>
   <si>
-    <t>PREFLABEL_FI</t>
-  </si>
-  <si>
-    <t>PREFLABEL_EN</t>
-  </si>
-  <si>
-    <t>STARTDATE</t>
-  </si>
-  <si>
-    <t>ENDDATE</t>
-  </si>
-  <si>
     <t>CREATED</t>
   </si>
   <si>
@@ -62,13 +83,19 @@
     <t>CODESSHEET</t>
   </si>
   <si>
+    <t>BROADER</t>
+  </si>
+  <si>
     <t>EXTENSIONSSHEET</t>
   </si>
   <si>
-    <t>BROADER</t>
-  </si>
-  <si>
-    <t>O1234567890123456789012345678901234567111</t>
+    <t>SHORTNAME</t>
+  </si>
+  <si>
+    <t>HIERARCHYLEVEL</t>
+  </si>
+  <si>
+    <t>ORDER</t>
   </si>
   <si>
     <t>P9;P1</t>
@@ -77,42 +104,24 @@
     <t>v1</t>
   </si>
   <si>
-    <t>DRAFT</t>
-  </si>
-  <si>
-    <t>SHORTNAME</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>testcode06</t>
   </si>
   <si>
-    <t>HIERARCHYLEVEL</t>
-  </si>
-  <si>
     <t>Testikoodisto2 pitkillä arvoilla</t>
   </si>
   <si>
-    <t>ORDER</t>
-  </si>
-  <si>
     <t>Test codescheme2 with long names</t>
   </si>
   <si>
     <t>2016-12-31</t>
   </si>
   <si>
-    <t>PROPERTYTYPE</t>
-  </si>
-  <si>
     <t>2018-12-30</t>
   </si>
   <si>
-    <t>CODESCHEMES</t>
-  </si>
-  <si>
     <t>2018-05-25</t>
   </si>
   <si>
@@ -122,15 +131,6 @@
     <t>Extensions_O1234567890111</t>
   </si>
   <si>
-    <t>MEMBERSSHEET</t>
-  </si>
-  <si>
-    <t>definitionHierarchy</t>
-  </si>
-  <si>
-    <t>http://uri.suomi.fi/codelist/eu/dcat</t>
-  </si>
-  <si>
     <t>testcode01</t>
   </si>
   <si>
@@ -158,12 +158,12 @@
     <t>Testilaajennus11</t>
   </si>
   <si>
+    <t>Test extension11</t>
+  </si>
+  <si>
     <t>testcode03</t>
   </si>
   <si>
-    <t>Test extension11</t>
-  </si>
-  <si>
     <t>Members_O12345678901234_3</t>
   </si>
   <si>
@@ -188,12 +188,12 @@
     <t>testcode04</t>
   </si>
   <si>
+    <t>Testikoodi 04</t>
+  </si>
+  <si>
     <t>Members_O12345678901234_4</t>
   </si>
   <si>
-    <t>Testikoodi 04</t>
-  </si>
-  <si>
     <t>Test code 04</t>
   </si>
   <si>
@@ -458,23 +458,56 @@
     <t>RELATION</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>y</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Jäsen1</t>
+  </si>
+  <si>
+    <t>Jäsen2</t>
+  </si>
+  <si>
+    <t>Jäsen3</t>
+  </si>
+  <si>
+    <t>Jäsen4</t>
+  </si>
+  <si>
+    <t>Jäsen5</t>
+  </si>
+  <si>
+    <t>Jäsen6</t>
+  </si>
+  <si>
+    <t>Jäsen7</t>
+  </si>
+  <si>
+    <t>Jäsen8</t>
+  </si>
+  <si>
+    <t>Jäsen9</t>
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/eu/dcat/EDUC</t>
   </si>
   <si>
+    <t>EDUC</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/eu/dcat/AGRI</t>
+  </si>
+  <si>
+    <t>AGRI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -490,6 +523,10 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF282828"/>
       <name val="Source Sans Pro"/>
@@ -509,16 +546,13 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <right/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -537,8 +571,11 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,99 +627,99 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
@@ -1706,31 +1743,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -1738,10 +1775,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
@@ -1750,7 +1787,7 @@
         <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>41</v>
@@ -1759,10 +1796,10 @@
         <v>41</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -1770,10 +1807,10 @@
         <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>43</v>
@@ -1782,7 +1819,7 @@
         <v>44</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>41</v>
@@ -1791,21 +1828,21 @@
         <v>45</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>50</v>
@@ -1814,7 +1851,7 @@
         <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>41</v>
@@ -1823,10 +1860,10 @@
         <v>53</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -1834,19 +1871,19 @@
         <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>41</v>
@@ -1855,10 +1892,10 @@
         <v>60</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -1866,10 +1903,10 @@
         <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>62</v>
@@ -1878,7 +1915,7 @@
         <v>63</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>41</v>
@@ -1887,21 +1924,21 @@
         <v>64</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>65</v>
@@ -1910,7 +1947,7 @@
         <v>66</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>41</v>
@@ -1919,10 +1956,10 @@
         <v>67</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -1930,10 +1967,10 @@
         <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>69</v>
@@ -1942,7 +1979,7 @@
         <v>70</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>41</v>
@@ -1951,10 +1988,10 @@
         <v>71</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -1962,10 +1999,10 @@
         <v>72</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>73</v>
@@ -1974,7 +2011,7 @@
         <v>74</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>41</v>
@@ -1983,10 +2020,10 @@
         <v>75</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -1994,10 +2031,10 @@
         <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>77</v>
@@ -2006,7 +2043,7 @@
         <v>78</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>41</v>
@@ -2015,10 +2052,10 @@
         <v>79</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -2026,10 +2063,10 @@
         <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>81</v>
@@ -2038,7 +2075,7 @@
         <v>82</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>41</v>
@@ -2047,10 +2084,10 @@
         <v>83</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -2058,10 +2095,10 @@
         <v>84</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>85</v>
@@ -2070,7 +2107,7 @@
         <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>41</v>
@@ -2079,10 +2116,10 @@
         <v>87</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -2090,10 +2127,10 @@
         <v>88</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>89</v>
@@ -2102,7 +2139,7 @@
         <v>90</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>41</v>
@@ -2111,10 +2148,10 @@
         <v>91</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -2122,10 +2159,10 @@
         <v>92</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>93</v>
@@ -2134,7 +2171,7 @@
         <v>94</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>41</v>
@@ -2143,10 +2180,10 @@
         <v>95</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -2154,10 +2191,10 @@
         <v>96</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>97</v>
@@ -2166,7 +2203,7 @@
         <v>98</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>41</v>
@@ -2175,10 +2212,10 @@
         <v>99</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -2186,10 +2223,10 @@
         <v>100</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>101</v>
@@ -2198,7 +2235,7 @@
         <v>102</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>41</v>
@@ -2207,10 +2244,10 @@
         <v>103</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -2218,10 +2255,10 @@
         <v>104</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>105</v>
@@ -2230,7 +2267,7 @@
         <v>106</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>41</v>
@@ -2239,10 +2276,10 @@
         <v>107</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -2250,10 +2287,10 @@
         <v>108</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>109</v>
@@ -2262,7 +2299,7 @@
         <v>110</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>41</v>
@@ -2271,10 +2308,10 @@
         <v>111</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
@@ -2282,10 +2319,10 @@
         <v>112</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>113</v>
@@ -2294,7 +2331,7 @@
         <v>114</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>41</v>
@@ -2303,10 +2340,10 @@
         <v>115</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -2314,10 +2351,10 @@
         <v>116</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>117</v>
@@ -2326,7 +2363,7 @@
         <v>118</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>41</v>
@@ -2335,10 +2372,10 @@
         <v>119</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -2346,10 +2383,10 @@
         <v>120</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>121</v>
@@ -2358,7 +2395,7 @@
         <v>122</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>41</v>
@@ -2367,10 +2404,10 @@
         <v>123</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -2378,10 +2415,10 @@
         <v>124</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>125</v>
@@ -2390,7 +2427,7 @@
         <v>126</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>41</v>
@@ -2399,10 +2436,10 @@
         <v>127</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -2410,10 +2447,10 @@
         <v>128</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>129</v>
@@ -2422,7 +2459,7 @@
         <v>130</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>41</v>
@@ -2431,10 +2468,10 @@
         <v>131</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -2442,10 +2479,10 @@
         <v>132</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>133</v>
@@ -2454,7 +2491,7 @@
         <v>134</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>41</v>
@@ -2463,10 +2500,10 @@
         <v>135</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -2474,10 +2511,10 @@
         <v>136</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>137</v>
@@ -2486,7 +2523,7 @@
         <v>138</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>41</v>
@@ -2495,10 +2532,10 @@
         <v>139</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -2506,10 +2543,10 @@
         <v>140</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>141</v>
@@ -2518,7 +2555,7 @@
         <v>142</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>41</v>
@@ -2527,10 +2564,10 @@
         <v>143</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1"/>
@@ -3535,54 +3572,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>49</v>
@@ -3593,13 +3630,13 @@
         <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>54</v>
@@ -3608,13 +3645,13 @@
         <v>55</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
@@ -4632,7 +4669,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.43"/>
+    <col customWidth="1" min="2" max="2" width="41.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4642,120 +4679,150 @@
       <c r="B1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="C2" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="5">
+      <c r="C3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="5">
         <v>3.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="5">
+      <c r="C5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="5">
         <v>4.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="5">
+      <c r="C6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="5">
         <v>5.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="5">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="5">
         <v>6.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="5">
+      <c r="C8" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="5">
         <v>7.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="5">
+        <v>158</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="5">
         <v>8.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="5">
+        <v>160</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="5">
         <v>9.0</v>
       </c>
     </row>
@@ -4788,120 +4855,150 @@
       <c r="B1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="C2" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="5">
+      <c r="C3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5">
+      <c r="C4" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="5">
         <v>3.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="5">
+      <c r="C5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="5">
         <v>4.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="5">
+      <c r="C6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="5">
         <v>5.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="5">
+      <c r="C7" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="5">
         <v>6.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="5">
+      <c r="C8" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="5">
         <v>7.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="5">
+      <c r="C9" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="5">
         <v>8.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="5">
+      <c r="C10" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="5">
         <v>9.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test cases 600-602 modified
</commit_message>
<xml_diff>
--- a/test_files/Codelist_with_def_hierarchy_extensions_and_members.xlsx
+++ b/test_files/Codelist_with_def_hierarchy_extensions_and_members.xlsx
@@ -15,32 +15,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="175">
   <si>
     <t>CODEVALUE</t>
   </si>
   <si>
+    <t>BROADER</t>
+  </si>
+  <si>
     <t>STATUS</t>
   </si>
   <si>
+    <t>PREFLABEL_FI</t>
+  </si>
+  <si>
+    <t>PREFLABEL_EN</t>
+  </si>
+  <si>
+    <t>SHORTNAME</t>
+  </si>
+  <si>
+    <t>HIERARCHYLEVEL</t>
+  </si>
+  <si>
+    <t>ORDER</t>
+  </si>
+  <si>
+    <t>STARTDATE</t>
+  </si>
+  <si>
+    <t>ENDDATE</t>
+  </si>
+  <si>
     <t>PROPERTYTYPE</t>
   </si>
   <si>
     <t>CODESCHEMES</t>
   </si>
   <si>
-    <t>PREFLABEL_FI</t>
-  </si>
-  <si>
-    <t>PREFLABEL_EN</t>
-  </si>
-  <si>
-    <t>STARTDATE</t>
-  </si>
-  <si>
-    <t>ENDDATE</t>
-  </si>
-  <si>
     <t>MEMBERSSHEET</t>
   </si>
   <si>
@@ -56,12 +68,63 @@
     <t>http://uri.suomi.fi/codelist/eu/dcat</t>
   </si>
   <si>
+    <t>testcode01</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Testikoodi 01</t>
+  </si>
+  <si>
+    <t>Test code 01</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Testilaajennus11</t>
+  </si>
+  <si>
+    <t>Test extension11</t>
+  </si>
+  <si>
+    <t>2016-12-31</t>
+  </si>
+  <si>
+    <t>2018-12-30</t>
+  </si>
+  <si>
+    <t>Members_O12345678901234_3</t>
+  </si>
+  <si>
+    <t>O1234567890123456789012345678901234567222</t>
+  </si>
+  <si>
+    <t>Testilaajennus22</t>
+  </si>
+  <si>
+    <t>Test extension22</t>
+  </si>
+  <si>
+    <t>Members_O12345678901234_4</t>
+  </si>
+  <si>
+    <t>testcode02</t>
+  </si>
+  <si>
     <t>CLASSIFICATION</t>
   </si>
   <si>
     <t>VERSION</t>
   </si>
   <si>
+    <t>Testikoodi 02</t>
+  </si>
+  <si>
+    <t>Test code 02</t>
+  </si>
+  <si>
     <t>SOURCE</t>
   </si>
   <si>
@@ -74,37 +137,55 @@
     <t>DEFAULTCODE</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>CREATED</t>
   </si>
   <si>
+    <t>testcode03</t>
+  </si>
+  <si>
     <t>MODIFIED</t>
   </si>
   <si>
     <t>CODESSHEET</t>
   </si>
   <si>
-    <t>BROADER</t>
+    <t>Testikoodi 03</t>
   </si>
   <si>
     <t>EXTENSIONSSHEET</t>
   </si>
   <si>
-    <t>SHORTNAME</t>
-  </si>
-  <si>
-    <t>HIERARCHYLEVEL</t>
-  </si>
-  <si>
-    <t>ORDER</t>
-  </si>
-  <si>
-    <t>P9;P1</t>
+    <t>Test code 03</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>P9;P1;P2</t>
+  </si>
+  <si>
+    <t>testcode04</t>
+  </si>
+  <si>
+    <t>Testikoodi 04</t>
+  </si>
+  <si>
+    <t>Test code 04</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>testcode05</t>
   </si>
   <si>
     <t>v1</t>
   </si>
   <si>
-    <t/>
+    <t>Testikoodi 05</t>
   </si>
   <si>
     <t>testcode06</t>
@@ -113,105 +194,24 @@
     <t>Testikoodisto2 pitkillä arvoilla</t>
   </si>
   <si>
+    <t>Test code 05</t>
+  </si>
+  <si>
     <t>Test codescheme2 with long names</t>
   </si>
   <si>
-    <t>2016-12-31</t>
-  </si>
-  <si>
-    <t>2018-12-30</t>
-  </si>
-  <si>
     <t>2018-05-25</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Codes_O123456789012345678901111</t>
   </si>
   <si>
     <t>Extensions_O1234567890111</t>
   </si>
   <si>
-    <t>testcode01</t>
-  </si>
-  <si>
-    <t>Testikoodi 01</t>
-  </si>
-  <si>
-    <t>Test code 01</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>testcode02</t>
-  </si>
-  <si>
-    <t>Testikoodi 02</t>
-  </si>
-  <si>
-    <t>Test code 02</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Testilaajennus11</t>
-  </si>
-  <si>
-    <t>Test extension11</t>
-  </si>
-  <si>
-    <t>testcode03</t>
-  </si>
-  <si>
-    <t>Members_O12345678901234_3</t>
-  </si>
-  <si>
-    <t>Testikoodi 03</t>
-  </si>
-  <si>
-    <t>Test code 03</t>
-  </si>
-  <si>
-    <t>O1234567890123456789012345678901234567222</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Testilaajennus22</t>
-  </si>
-  <si>
-    <t>Test extension22</t>
-  </si>
-  <si>
-    <t>testcode04</t>
-  </si>
-  <si>
-    <t>Testikoodi 04</t>
-  </si>
-  <si>
-    <t>Members_O12345678901234_4</t>
-  </si>
-  <si>
-    <t>Test code 04</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>testcode05</t>
-  </si>
-  <si>
-    <t>Testikoodi 05</t>
-  </si>
-  <si>
-    <t>Test code 05</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>Testikoodi 06</t>
   </si>
   <si>
@@ -449,6 +449,18 @@
     <t>25</t>
   </si>
   <si>
+    <t>UNARYOPERATOR</t>
+  </si>
+  <si>
+    <t>UNARYOPERATIR</t>
+  </si>
+  <si>
+    <t>COMPARISONOPERATOR</t>
+  </si>
+  <si>
+    <t>MEMBERVALUE_3</t>
+  </si>
+  <si>
     <t>MEMBERVALUE_1</t>
   </si>
   <si>
@@ -467,47 +479,77 @@
     <t>Jäsen1</t>
   </si>
   <si>
+    <t>Member1</t>
+  </si>
+  <si>
     <t>Jäsen2</t>
   </si>
   <si>
+    <t>Member2</t>
+  </si>
+  <si>
     <t>Jäsen3</t>
   </si>
   <si>
+    <t>Member3</t>
+  </si>
+  <si>
     <t>Jäsen4</t>
   </si>
   <si>
+    <t>Member4</t>
+  </si>
+  <si>
     <t>Jäsen5</t>
   </si>
   <si>
+    <t>Member5</t>
+  </si>
+  <si>
     <t>Jäsen6</t>
   </si>
   <si>
+    <t>Member6</t>
+  </si>
+  <si>
     <t>Jäsen7</t>
   </si>
   <si>
+    <t>Member7</t>
+  </si>
+  <si>
     <t>Jäsen8</t>
   </si>
   <si>
+    <t>Member8</t>
+  </si>
+  <si>
     <t>Jäsen9</t>
   </si>
   <si>
+    <t>Member9</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/eu/dcat/EDUC</t>
   </si>
   <si>
-    <t>EDUC</t>
+    <t>educ</t>
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/eu/dcat/AGRI</t>
   </si>
   <si>
-    <t>AGRI</t>
+    <t>agri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -521,12 +563,15 @@
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <sz val="11.0"/>
+      <color rgb="FF282828"/>
+      <name val="Source Sans Pro"/>
     </font>
     <font>
+      <u/>
       <sz val="11.0"/>
       <color rgb="FF282828"/>
       <name val="Source Sans Pro"/>
@@ -552,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -565,17 +610,29 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,9 +673,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="41.29"/>
-    <col customWidth="1" min="2" max="6" width="14.43"/>
+    <col customWidth="1" min="2" max="2" width="21.86"/>
+    <col customWidth="1" min="3" max="6" width="14.43"/>
     <col customWidth="1" min="10" max="10" width="23.71"/>
-    <col customWidth="1" min="15" max="15" width="18.57"/>
+    <col customWidth="1" min="15" max="15" width="30.43"/>
     <col customWidth="1" min="16" max="16" width="29.29"/>
   </cols>
   <sheetData>
@@ -627,99 +685,99 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>35</v>
+        <v>61</v>
+      </c>
+      <c r="N2" s="4">
+        <v>43976.0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
@@ -1735,7 +1793,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="14.43"/>
+    <col customWidth="1" min="1" max="3" width="14.43"/>
+    <col customWidth="1" min="4" max="4" width="19.57"/>
+    <col customWidth="1" min="5" max="5" width="19.86"/>
+    <col customWidth="1" min="6" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1743,202 +1804,202 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="I2" s="4">
+        <v>43101.0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>43831.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
+      </c>
+      <c r="I3" s="4">
+        <v>43102.0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>43832.0</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>29</v>
+      <c r="I4" s="4">
+        <v>43103.0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>43833.0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
+      </c>
+      <c r="I5" s="4">
+        <v>43104.0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>43834.0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>29</v>
+      <c r="I6" s="4">
+        <v>43105.0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>43835.0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>65</v>
@@ -1947,19 +2008,19 @@
         <v>66</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>29</v>
+      <c r="I7" s="4">
+        <v>43106.0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>43836.0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -1967,10 +2028,10 @@
         <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>69</v>
@@ -1979,19 +2040,19 @@
         <v>70</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>29</v>
+      <c r="I8" s="4">
+        <v>43107.0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>43837.0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -1999,10 +2060,10 @@
         <v>72</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>73</v>
@@ -2011,19 +2072,19 @@
         <v>74</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>29</v>
+      <c r="I9" s="4">
+        <v>43108.0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>43838.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -2031,10 +2092,10 @@
         <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>77</v>
@@ -2043,19 +2104,19 @@
         <v>78</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>29</v>
+      <c r="I10" s="4">
+        <v>43109.0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>43839.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -2063,10 +2124,10 @@
         <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>81</v>
@@ -2075,19 +2136,19 @@
         <v>82</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>29</v>
+      <c r="I11" s="4">
+        <v>43110.0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>43840.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -2095,10 +2156,10 @@
         <v>84</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>85</v>
@@ -2107,19 +2168,19 @@
         <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>29</v>
+      <c r="I12" s="4">
+        <v>43111.0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>43841.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -2127,10 +2188,10 @@
         <v>88</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>89</v>
@@ -2139,19 +2200,19 @@
         <v>90</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>29</v>
+      <c r="I13" s="4">
+        <v>43112.0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>43842.0</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -2159,10 +2220,10 @@
         <v>92</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>93</v>
@@ -2171,19 +2232,19 @@
         <v>94</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>29</v>
+      <c r="I14" s="4">
+        <v>43113.0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>43843.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -2191,10 +2252,10 @@
         <v>96</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>97</v>
@@ -2203,19 +2264,19 @@
         <v>98</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>29</v>
+      <c r="I15" s="4">
+        <v>43114.0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>43844.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -2223,10 +2284,10 @@
         <v>100</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>101</v>
@@ -2235,19 +2296,19 @@
         <v>102</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>29</v>
+      <c r="I16" s="4">
+        <v>43115.0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>43845.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -2255,10 +2316,10 @@
         <v>104</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>105</v>
@@ -2267,19 +2328,19 @@
         <v>106</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>29</v>
+      <c r="I17" s="4">
+        <v>43116.0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>43846.0</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -2287,10 +2348,10 @@
         <v>108</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>109</v>
@@ -2299,19 +2360,19 @@
         <v>110</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>29</v>
+      <c r="I18" s="4">
+        <v>43117.0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>43847.0</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
@@ -2319,10 +2380,10 @@
         <v>112</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>113</v>
@@ -2331,19 +2392,19 @@
         <v>114</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>29</v>
+      <c r="I19" s="4">
+        <v>43118.0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>43848.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -2351,10 +2412,10 @@
         <v>116</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>117</v>
@@ -2363,19 +2424,19 @@
         <v>118</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>29</v>
+      <c r="I20" s="4">
+        <v>43119.0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>43849.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -2383,10 +2444,10 @@
         <v>120</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>121</v>
@@ -2395,19 +2456,19 @@
         <v>122</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>29</v>
+      <c r="I21" s="4">
+        <v>43120.0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>43850.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -2415,10 +2476,10 @@
         <v>124</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>125</v>
@@ -2427,19 +2488,19 @@
         <v>126</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>29</v>
+      <c r="I22" s="4">
+        <v>43121.0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>43851.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -2447,10 +2508,10 @@
         <v>128</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>129</v>
@@ -2459,19 +2520,19 @@
         <v>130</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>29</v>
+      <c r="I23" s="4">
+        <v>43122.0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>43852.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -2479,10 +2540,10 @@
         <v>132</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>133</v>
@@ -2491,19 +2552,19 @@
         <v>134</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>29</v>
+      <c r="I24" s="4">
+        <v>43123.0</v>
+      </c>
+      <c r="J24" s="4">
+        <v>43853.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -2511,10 +2572,10 @@
         <v>136</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>137</v>
@@ -2523,19 +2584,19 @@
         <v>138</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>29</v>
+      <c r="I25" s="4">
+        <v>43124.0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>43854.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -2543,10 +2604,10 @@
         <v>140</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>141</v>
@@ -2555,19 +2616,19 @@
         <v>142</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>29</v>
+      <c r="I26" s="4">
+        <v>43125.0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>43855.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1"/>
@@ -3562,7 +3623,8 @@
     <col customWidth="1" min="1" max="1" width="45.29"/>
     <col customWidth="1" min="2" max="2" width="14.43"/>
     <col customWidth="1" min="3" max="3" width="23.71"/>
-    <col customWidth="1" min="4" max="5" width="27.0"/>
+    <col customWidth="1" min="4" max="4" width="40.57"/>
+    <col customWidth="1" min="5" max="5" width="27.0"/>
     <col customWidth="1" min="6" max="6" width="26.57"/>
     <col customWidth="1" min="9" max="9" width="29.29"/>
   </cols>
@@ -3572,86 +3634,86 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
@@ -4669,167 +4731,321 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="20.14"/>
     <col customWidth="1" min="2" max="2" width="41.86"/>
+    <col customWidth="1" min="3" max="3" width="21.0"/>
+    <col customWidth="1" min="4" max="4" width="57.14"/>
+    <col customWidth="1" min="5" max="5" width="21.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
+      <c r="G1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="A2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8">
         <v>1.0</v>
+      </c>
+      <c r="I2" s="9">
+        <v>43101.0</v>
+      </c>
+      <c r="J2" s="9">
+        <v>43831.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="5">
+      <c r="A3" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="8">
         <v>2.0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>43102.0</v>
+      </c>
+      <c r="J3" s="9">
+        <v>43832.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="5">
+      <c r="B4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="8">
         <v>3.0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>43103.0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>43833.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="5">
+      <c r="C5" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="8">
         <v>4.0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>43104.0</v>
+      </c>
+      <c r="J5" s="9">
+        <v>43834.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="5">
+      <c r="A6" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="8">
         <v>5.0</v>
+      </c>
+      <c r="I6" s="9">
+        <v>43105.0</v>
+      </c>
+      <c r="J6" s="9">
+        <v>43835.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="5">
+      <c r="A7" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="8">
         <v>6.0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>43106.0</v>
+      </c>
+      <c r="J7" s="9">
+        <v>43836.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="5">
+      <c r="E8" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="8">
         <v>7.0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>43107.0</v>
+      </c>
+      <c r="J8" s="9">
+        <v>43837.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>148</v>
+      <c r="A9" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="5">
+        <v>152</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="8">
         <v>8.0</v>
+      </c>
+      <c r="I9" s="9">
+        <v>43108.0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>43838.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>148</v>
+      <c r="A10" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="5">
+        <v>152</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="8">
         <v>9.0</v>
+      </c>
+      <c r="I10" s="9">
+        <v>43109.0</v>
+      </c>
+      <c r="J10" s="9">
+        <v>43839.0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B9"/>
-    <hyperlink r:id="rId2" ref="B10"/>
+    <hyperlink r:id="rId1" ref="D9"/>
+    <hyperlink r:id="rId2" ref="D10"/>
   </hyperlinks>
   <drawing r:id="rId3"/>
 </worksheet>
@@ -4845,161 +5061,311 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.43"/>
+    <col customWidth="1" min="1" max="3" width="34.43"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
+      <c r="G1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="E2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8">
         <v>1.0</v>
+      </c>
+      <c r="I2" s="9">
+        <v>43101.0</v>
+      </c>
+      <c r="J2" s="9">
+        <v>43831.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="5">
+      <c r="E3" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="8">
         <v>2.0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>43102.0</v>
+      </c>
+      <c r="J3" s="9">
+        <v>43832.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="5">
+      <c r="E4" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="8">
         <v>3.0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>43103.0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>43833.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="5">
+      <c r="E5" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="8">
         <v>4.0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>43104.0</v>
+      </c>
+      <c r="J5" s="9">
+        <v>43834.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="5">
+      <c r="E6" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="8">
         <v>5.0</v>
+      </c>
+      <c r="I6" s="9">
+        <v>43105.0</v>
+      </c>
+      <c r="J6" s="9">
+        <v>43835.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="5">
+      <c r="E7" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="8">
         <v>6.0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>43106.0</v>
+      </c>
+      <c r="J7" s="9">
+        <v>43836.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="5">
+      <c r="E8" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="8">
         <v>7.0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>43107.0</v>
+      </c>
+      <c r="J8" s="9">
+        <v>43837.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="5">
+      <c r="E9" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="8">
         <v>8.0</v>
+      </c>
+      <c r="I9" s="9">
+        <v>43108.0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>43838.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="5">
+      <c r="E10" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="8">
         <v>9.0</v>
+      </c>
+      <c r="I10" s="9">
+        <v>43109.0</v>
+      </c>
+      <c r="J10" s="9">
+        <v>43839.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>